<commit_message>
added tags and challenges to editable fields
</commit_message>
<xml_diff>
--- a/Badge-List-102016.xlsx
+++ b/Badge-List-102016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="12" windowWidth="23256" windowHeight="12912"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -3546,8 +3546,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3613,6 +3613,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3691,6 +3696,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3725,6 +3731,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3900,22 +3907,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="D248" sqref="D248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="1" customWidth="1"/>
-    <col min="5" max="8" width="23.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.109375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="23.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1027</v>
       </c>
@@ -3941,7 +3948,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="76.5">
+    <row r="2" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>541</v>
       </c>
@@ -3967,7 +3974,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="51">
+    <row r="3" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>537</v>
       </c>
@@ -3993,7 +4000,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="51">
+    <row r="4" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -4019,7 +4026,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="38.25">
+    <row r="5" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>533</v>
       </c>
@@ -4045,7 +4052,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="38.25">
+    <row r="6" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>529</v>
       </c>
@@ -4071,7 +4078,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="63.75">
+    <row r="7" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>590</v>
       </c>
@@ -4097,7 +4104,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51">
+    <row r="8" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>586</v>
       </c>
@@ -4123,7 +4130,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="178.5">
+    <row r="9" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>525</v>
       </c>
@@ -4149,7 +4156,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="51">
+    <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>237</v>
       </c>
@@ -4175,7 +4182,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="38.25">
+    <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>582</v>
       </c>
@@ -4201,7 +4208,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="51">
+    <row r="12" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
@@ -4227,7 +4234,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="76.5">
+    <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>147</v>
       </c>
@@ -4253,7 +4260,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="229.5">
+    <row r="14" spans="1:8" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
@@ -4279,7 +4286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="102">
+    <row r="15" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>120</v>
       </c>
@@ -4305,7 +4312,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="51">
+    <row r="16" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1006</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="38.25">
+    <row r="17" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1003</v>
       </c>
@@ -4357,7 +4364,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="51">
+    <row r="18" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>813</v>
       </c>
@@ -4383,7 +4390,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="178.5">
+    <row r="19" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -4409,7 +4416,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="63.75">
+    <row r="20" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
@@ -4435,7 +4442,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="51">
+    <row r="21" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>884</v>
       </c>
@@ -4461,7 +4468,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="89.25">
+    <row r="22" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>891</v>
       </c>
@@ -4487,7 +4494,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="51">
+    <row r="23" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>521</v>
       </c>
@@ -4513,7 +4520,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="38.25">
+    <row r="24" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>518</v>
       </c>
@@ -4539,7 +4546,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="38.25">
+    <row r="25" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>515</v>
       </c>
@@ -4565,7 +4572,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="63.75">
+    <row r="26" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>80</v>
       </c>
@@ -4591,7 +4598,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="127.5">
+    <row r="27" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>205</v>
       </c>
@@ -4617,7 +4624,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="51">
+    <row r="28" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>512</v>
       </c>
@@ -4643,7 +4650,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="51">
+    <row r="29" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>510</v>
       </c>
@@ -4669,7 +4676,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="76.5">
+    <row r="30" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>507</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="89.25">
+    <row r="31" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>504</v>
       </c>
@@ -4721,7 +4728,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="38.25">
+    <row r="32" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>881</v>
       </c>
@@ -4747,7 +4754,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="102">
+    <row r="33" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>501</v>
       </c>
@@ -4773,7 +4780,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="38.25">
+    <row r="34" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>685</v>
       </c>
@@ -4799,7 +4806,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="63.75">
+    <row r="35" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>832</v>
       </c>
@@ -4825,7 +4832,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="38.25">
+    <row r="36" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1000</v>
       </c>
@@ -4851,7 +4858,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="63.75">
+    <row r="37" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>791</v>
       </c>
@@ -4877,7 +4884,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="51">
+    <row r="38" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>888</v>
       </c>
@@ -4903,7 +4910,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="204">
+    <row r="39" spans="1:8" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>233</v>
       </c>
@@ -4929,7 +4936,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="38.25">
+    <row r="40" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>498</v>
       </c>
@@ -4955,7 +4962,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="127.5">
+    <row r="41" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>495</v>
       </c>
@@ -4981,7 +4988,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="51">
+    <row r="42" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>492</v>
       </c>
@@ -5007,7 +5014,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="63.75">
+    <row r="43" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>107</v>
       </c>
@@ -5033,7 +5040,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="63.75">
+    <row r="44" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>878</v>
       </c>
@@ -5059,7 +5066,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="38.25">
+    <row r="45" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
@@ -5085,7 +5092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="51">
+    <row r="46" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>245</v>
       </c>
@@ -5111,7 +5118,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="51">
+    <row r="47" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>192</v>
       </c>
@@ -5137,7 +5144,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="38.25">
+    <row r="48" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
@@ -5163,7 +5170,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="51">
+    <row r="49" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>202</v>
       </c>
@@ -5189,7 +5196,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="114.75">
+    <row r="50" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>682</v>
       </c>
@@ -5215,7 +5222,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="63.75">
+    <row r="51" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>199</v>
       </c>
@@ -5241,7 +5248,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="63.75">
+    <row r="52" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>788</v>
       </c>
@@ -5267,7 +5274,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="38.25">
+    <row r="53" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>489</v>
       </c>
@@ -5293,7 +5300,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="76.5">
+    <row r="54" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>486</v>
       </c>
@@ -5319,7 +5326,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="38.25">
+    <row r="55" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>73</v>
       </c>
@@ -5345,7 +5352,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="51">
+    <row r="56" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>483</v>
       </c>
@@ -5371,7 +5378,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="38.25">
+    <row r="57" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>480</v>
       </c>
@@ -5397,7 +5404,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="76.5">
+    <row r="58" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>189</v>
       </c>
@@ -5423,7 +5430,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="102">
+    <row r="59" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
@@ -5449,7 +5456,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="63.75">
+    <row r="60" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>230</v>
       </c>
@@ -5475,7 +5482,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="63.75">
+    <row r="61" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>785</v>
       </c>
@@ -5501,7 +5508,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="38.25">
+    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>477</v>
       </c>
@@ -5527,7 +5534,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="204">
+    <row r="63" spans="1:8" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>810</v>
       </c>
@@ -5553,7 +5560,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="51">
+    <row r="64" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>474</v>
       </c>
@@ -5579,7 +5586,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="255">
+    <row r="65" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>104</v>
       </c>
@@ -5605,7 +5612,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="229.5">
+    <row r="66" spans="1:8" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>471</v>
       </c>
@@ -5631,7 +5638,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="38.25">
+    <row r="67" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>640</v>
       </c>
@@ -5657,7 +5664,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="76.5">
+    <row r="68" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>468</v>
       </c>
@@ -5683,7 +5690,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="51">
+    <row r="69" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>465</v>
       </c>
@@ -5709,7 +5716,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="63.75">
+    <row r="70" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>782</v>
       </c>
@@ -5735,7 +5742,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="204">
+    <row r="71" spans="1:8" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>186</v>
       </c>
@@ -5761,7 +5768,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="191.25">
+    <row r="72" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>184</v>
       </c>
@@ -5787,7 +5794,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="51">
+    <row r="73" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>462</v>
       </c>
@@ -5813,7 +5820,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="38.25">
+    <row r="74" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>997</v>
       </c>
@@ -5839,7 +5846,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="51">
+    <row r="75" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>875</v>
       </c>
@@ -5865,7 +5872,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="38.25">
+    <row r="76" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>679</v>
       </c>
@@ -5891,7 +5898,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="51">
+    <row r="77" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>70</v>
       </c>
@@ -5917,7 +5924,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="63.75">
+    <row r="78" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>459</v>
       </c>
@@ -5943,7 +5950,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="51">
+    <row r="79" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>779</v>
       </c>
@@ -5969,7 +5976,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="51">
+    <row r="80" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>578</v>
       </c>
@@ -5995,7 +6002,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="51">
+    <row r="81" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>776</v>
       </c>
@@ -6021,7 +6028,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="165.75">
+    <row r="82" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>456</v>
       </c>
@@ -6047,7 +6054,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="51">
+    <row r="83" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>994</v>
       </c>
@@ -6073,7 +6080,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="89.25">
+    <row r="84" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>807</v>
       </c>
@@ -6099,7 +6106,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="38.25">
+    <row r="85" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>773</v>
       </c>
@@ -6125,7 +6132,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="51">
+    <row r="86" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>770</v>
       </c>
@@ -6151,7 +6158,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="51">
+    <row r="87" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>453</v>
       </c>
@@ -6177,7 +6184,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="38.25">
+    <row r="88" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>767</v>
       </c>
@@ -6203,7 +6210,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="38.25">
+    <row r="89" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>211</v>
       </c>
@@ -6229,7 +6236,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="38.25">
+    <row r="90" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>209</v>
       </c>
@@ -6255,7 +6262,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="38.25">
+    <row r="91" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
@@ -6281,7 +6288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="38.25">
+    <row r="92" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>64</v>
       </c>
@@ -6307,7 +6314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="51">
+    <row r="93" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>1019</v>
       </c>
@@ -6333,7 +6340,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="51">
+    <row r="94" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>450</v>
       </c>
@@ -6359,7 +6366,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="127.5">
+    <row r="95" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>447</v>
       </c>
@@ -6385,7 +6392,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="76.5">
+    <row r="96" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>444</v>
       </c>
@@ -6411,7 +6418,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="204">
+    <row r="97" spans="1:8" ht="198" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>442</v>
       </c>
@@ -6437,7 +6444,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="51">
+    <row r="98" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>439</v>
       </c>
@@ -6463,7 +6470,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="38.25">
+    <row r="99" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>1016</v>
       </c>
@@ -6489,7 +6496,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="51">
+    <row r="100" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>144</v>
       </c>
@@ -6515,7 +6522,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="51">
+    <row r="101" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>676</v>
       </c>
@@ -6541,7 +6548,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="76.5">
+    <row r="102" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>436</v>
       </c>
@@ -6567,7 +6574,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="63.75">
+    <row r="103" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>434</v>
       </c>
@@ -6593,7 +6600,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="51">
+    <row r="104" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>764</v>
       </c>
@@ -6619,7 +6626,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="38.25">
+    <row r="105" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -6645,7 +6652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="51">
+    <row r="106" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>872</v>
       </c>
@@ -6671,7 +6678,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="51">
+    <row r="107" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>101</v>
       </c>
@@ -6697,7 +6704,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="63.75">
+    <row r="108" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>829</v>
       </c>
@@ -6723,7 +6730,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="38.25">
+    <row r="109" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>898</v>
       </c>
@@ -6749,7 +6756,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="38.25">
+    <row r="110" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>991</v>
       </c>
@@ -6775,7 +6782,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="51">
+    <row r="111" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>431</v>
       </c>
@@ -6801,7 +6808,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="38.25">
+    <row r="112" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>428</v>
       </c>
@@ -6827,7 +6834,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="89.25">
+    <row r="113" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>425</v>
       </c>
@@ -6853,7 +6860,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="51">
+    <row r="114" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>422</v>
       </c>
@@ -6879,7 +6886,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="38.25">
+    <row r="115" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>249</v>
       </c>
@@ -6905,7 +6912,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="63.75">
+    <row r="116" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>420</v>
       </c>
@@ -6931,7 +6938,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="51">
+    <row r="117" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>141</v>
       </c>
@@ -6957,7 +6964,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="102">
+    <row r="118" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>139</v>
       </c>
@@ -6983,7 +6990,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="38.25">
+    <row r="119" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>988</v>
       </c>
@@ -7009,7 +7016,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="51">
+    <row r="120" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>761</v>
       </c>
@@ -7035,7 +7042,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="51">
+    <row r="121" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>417</v>
       </c>
@@ -7061,7 +7068,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="51">
+    <row r="122" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>414</v>
       </c>
@@ -7087,7 +7094,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="127.5">
+    <row r="123" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>196</v>
       </c>
@@ -7113,7 +7120,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="38.25">
+    <row r="124" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>985</v>
       </c>
@@ -7139,7 +7146,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="114.75">
+    <row r="125" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>983</v>
       </c>
@@ -7165,7 +7172,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="38.25">
+    <row r="126" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>411</v>
       </c>
@@ -7191,7 +7198,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="51">
+    <row r="127" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>408</v>
       </c>
@@ -7217,7 +7224,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="38.25">
+    <row r="128" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>1013</v>
       </c>
@@ -7243,7 +7250,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="38.25">
+    <row r="129" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>869</v>
       </c>
@@ -7269,7 +7276,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="51">
+    <row r="130" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>758</v>
       </c>
@@ -7295,7 +7302,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="38.25">
+    <row r="131" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -7321,7 +7328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="38.25">
+    <row r="132" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>866</v>
       </c>
@@ -7347,7 +7354,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="38.25">
+    <row r="133" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>980</v>
       </c>
@@ -7373,7 +7380,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="38.25">
+    <row r="134" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>977</v>
       </c>
@@ -7399,7 +7406,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="38.25">
+    <row r="135" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>974</v>
       </c>
@@ -7425,7 +7432,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="102">
+    <row r="136" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>628</v>
       </c>
@@ -7451,7 +7458,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="38.25">
+    <row r="137" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>575</v>
       </c>
@@ -7477,7 +7484,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="38.25">
+    <row r="138" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>902</v>
       </c>
@@ -7503,7 +7510,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="38.25">
+    <row r="139" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>405</v>
       </c>
@@ -7529,7 +7536,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="51">
+    <row r="140" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>135</v>
       </c>
@@ -7555,7 +7562,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="38.25">
+    <row r="141" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>402</v>
       </c>
@@ -7581,7 +7588,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="51">
+    <row r="142" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>572</v>
       </c>
@@ -7607,7 +7614,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="38.25">
+    <row r="143" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>971</v>
       </c>
@@ -7633,7 +7640,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="76.5">
+    <row r="144" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>1010</v>
       </c>
@@ -7659,7 +7666,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="38.25">
+    <row r="145" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>61</v>
       </c>
@@ -7685,7 +7692,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="38.25">
+    <row r="146" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>968</v>
       </c>
@@ -7711,7 +7718,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="51">
+    <row r="147" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>895</v>
       </c>
@@ -7737,7 +7744,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="38.25">
+    <row r="148" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>58</v>
       </c>
@@ -7763,7 +7770,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="102">
+    <row r="149" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>181</v>
       </c>
@@ -7789,7 +7796,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="127.5">
+    <row r="150" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>673</v>
       </c>
@@ -7815,7 +7822,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="38.25">
+    <row r="151" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>965</v>
       </c>
@@ -7841,7 +7848,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="38.25">
+    <row r="152" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>755</v>
       </c>
@@ -7867,7 +7874,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="63.75">
+    <row r="153" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>753</v>
       </c>
@@ -7893,7 +7900,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="38.25">
+    <row r="154" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>569</v>
       </c>
@@ -7919,7 +7926,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="63.75">
+    <row r="155" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>750</v>
       </c>
@@ -7945,7 +7952,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="63.75">
+    <row r="156" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>55</v>
       </c>
@@ -7971,7 +7978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="51">
+    <row r="157" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>670</v>
       </c>
@@ -7997,7 +8004,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="51">
+    <row r="158" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>863</v>
       </c>
@@ -8023,7 +8030,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="38.25">
+    <row r="159" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>52</v>
       </c>
@@ -8049,7 +8056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="38.25">
+    <row r="160" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>49</v>
       </c>
@@ -8075,7 +8082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="63.75">
+    <row r="161" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>399</v>
       </c>
@@ -8101,7 +8108,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="51">
+    <row r="162" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>396</v>
       </c>
@@ -8127,7 +8134,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="38.25">
+    <row r="163" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>227</v>
       </c>
@@ -8153,7 +8160,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="63.75">
+    <row r="164" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>747</v>
       </c>
@@ -8179,7 +8186,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="38.25">
+    <row r="165" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>744</v>
       </c>
@@ -8205,7 +8212,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="89.25">
+    <row r="166" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>689</v>
       </c>
@@ -8231,7 +8238,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="357">
+    <row r="167" spans="1:8" ht="369.6" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>804</v>
       </c>
@@ -8257,7 +8264,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="38.25">
+    <row r="168" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>962</v>
       </c>
@@ -8283,7 +8290,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="38.25">
+    <row r="169" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>742</v>
       </c>
@@ -8309,7 +8316,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="38.25">
+    <row r="170" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>860</v>
       </c>
@@ -8335,7 +8342,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="38.25">
+    <row r="171" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>857</v>
       </c>
@@ -8361,7 +8368,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="127.5">
+    <row r="172" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>393</v>
       </c>
@@ -8387,7 +8394,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="38.25">
+    <row r="173" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>739</v>
       </c>
@@ -8413,7 +8420,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="51">
+    <row r="174" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>390</v>
       </c>
@@ -8439,7 +8446,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="76.5">
+    <row r="175" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>387</v>
       </c>
@@ -8465,7 +8472,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="51">
+    <row r="176" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>241</v>
       </c>
@@ -8491,7 +8498,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="38.25">
+    <row r="177" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>46</v>
       </c>
@@ -8517,7 +8524,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="38.25">
+    <row r="178" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>959</v>
       </c>
@@ -8543,7 +8550,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="51">
+    <row r="179" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>957</v>
       </c>
@@ -8569,7 +8576,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="38.25">
+    <row r="180" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>954</v>
       </c>
@@ -8595,7 +8602,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="38.25">
+    <row r="181" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>854</v>
       </c>
@@ -8621,7 +8628,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="51">
+    <row r="182" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>384</v>
       </c>
@@ -8647,7 +8654,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="51">
+    <row r="183" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>625</v>
       </c>
@@ -8673,7 +8680,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="38.25">
+    <row r="184" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>381</v>
       </c>
@@ -8699,7 +8706,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="38.25">
+    <row r="185" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>378</v>
       </c>
@@ -8725,7 +8732,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="51">
+    <row r="186" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>951</v>
       </c>
@@ -8751,7 +8758,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="51">
+    <row r="187" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>224</v>
       </c>
@@ -8777,7 +8784,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="204">
+    <row r="188" spans="1:8" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>375</v>
       </c>
@@ -8803,7 +8810,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="191.25">
+    <row r="189" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>373</v>
       </c>
@@ -8829,7 +8836,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="38.25">
+    <row r="190" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>566</v>
       </c>
@@ -8855,7 +8862,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="38.25">
+    <row r="191" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>736</v>
       </c>
@@ -8881,7 +8888,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="38.25">
+    <row r="192" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>734</v>
       </c>
@@ -8907,7 +8914,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="38.25">
+    <row r="193" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>621</v>
       </c>
@@ -8933,7 +8940,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="51">
+    <row r="194" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>370</v>
       </c>
@@ -8959,7 +8966,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="51">
+    <row r="195" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>826</v>
       </c>
@@ -8985,7 +8992,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="89.25">
+    <row r="196" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>178</v>
       </c>
@@ -9011,7 +9018,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="63.75">
+    <row r="197" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>367</v>
       </c>
@@ -9037,7 +9044,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="51">
+    <row r="198" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>364</v>
       </c>
@@ -9063,7 +9070,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="38.25">
+    <row r="199" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>132</v>
       </c>
@@ -9089,7 +9096,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="63.75">
+    <row r="200" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>618</v>
       </c>
@@ -9115,7 +9122,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="38.25">
+    <row r="201" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>563</v>
       </c>
@@ -9141,7 +9148,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="38.25">
+    <row r="202" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>43</v>
       </c>
@@ -9167,7 +9174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="51">
+    <row r="203" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>40</v>
       </c>
@@ -9193,7 +9200,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="51">
+    <row r="204" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>361</v>
       </c>
@@ -9219,7 +9226,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="140.25">
+    <row r="205" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>358</v>
       </c>
@@ -9245,7 +9252,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="51">
+    <row r="206" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>355</v>
       </c>
@@ -9271,7 +9278,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="51">
+    <row r="207" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>115</v>
       </c>
@@ -9297,7 +9304,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="38.25">
+    <row r="208" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>560</v>
       </c>
@@ -9323,7 +9330,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="63.75">
+    <row r="209" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>175</v>
       </c>
@@ -9349,7 +9356,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="38.25">
+    <row r="210" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>948</v>
       </c>
@@ -9375,7 +9382,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="63.75">
+    <row r="211" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>352</v>
       </c>
@@ -9401,7 +9408,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="89.25">
+    <row r="212" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>823</v>
       </c>
@@ -9427,7 +9434,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="38.25">
+    <row r="213" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>615</v>
       </c>
@@ -9453,7 +9460,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="38.25">
+    <row r="214" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>557</v>
       </c>
@@ -9479,7 +9486,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="51">
+    <row r="215" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>612</v>
       </c>
@@ -9505,7 +9512,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="280.5">
+    <row r="216" spans="1:8" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>154</v>
       </c>
@@ -9531,7 +9538,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="38.25">
+    <row r="217" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>731</v>
       </c>
@@ -9557,7 +9564,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="38.25">
+    <row r="218" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>729</v>
       </c>
@@ -9583,7 +9590,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="38.25">
+    <row r="219" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>851</v>
       </c>
@@ -9609,7 +9616,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="178.5">
+    <row r="220" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>98</v>
       </c>
@@ -9635,7 +9642,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="51">
+    <row r="221" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>96</v>
       </c>
@@ -9661,7 +9668,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="140.25">
+    <row r="222" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>93</v>
       </c>
@@ -9687,7 +9694,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="76.5">
+    <row r="223" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>604</v>
       </c>
@@ -9713,7 +9720,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="114.75">
+    <row r="224" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>848</v>
       </c>
@@ -9739,7 +9746,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="51">
+    <row r="225" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>726</v>
       </c>
@@ -9765,7 +9772,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="153">
+    <row r="226" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>724</v>
       </c>
@@ -9791,7 +9798,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="89.25">
+    <row r="227" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>722</v>
       </c>
@@ -9817,7 +9824,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="280.5">
+    <row r="228" spans="1:8" ht="290.39999999999998" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>349</v>
       </c>
@@ -9843,7 +9850,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="38.25">
+    <row r="229" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>667</v>
       </c>
@@ -9869,7 +9876,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="51">
+    <row r="230" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>665</v>
       </c>
@@ -9895,7 +9902,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="51">
+    <row r="231" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>663</v>
       </c>
@@ -9921,7 +9928,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="51">
+    <row r="232" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>719</v>
       </c>
@@ -9947,7 +9954,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="63.75">
+    <row r="233" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>37</v>
       </c>
@@ -9973,7 +9980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="51">
+    <row r="234" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>716</v>
       </c>
@@ -9999,7 +10006,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="38.25">
+    <row r="235" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>34</v>
       </c>
@@ -10025,7 +10032,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="51">
+    <row r="236" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>346</v>
       </c>
@@ -10051,7 +10058,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="89.25">
+    <row r="237" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>343</v>
       </c>
@@ -10077,7 +10084,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="63.75">
+    <row r="238" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>341</v>
       </c>
@@ -10103,7 +10110,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="38.25">
+    <row r="239" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>338</v>
       </c>
@@ -10129,7 +10136,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="38.25">
+    <row r="240" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>945</v>
       </c>
@@ -10155,7 +10162,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="38.25">
+    <row r="241" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>608</v>
       </c>
@@ -10181,7 +10188,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="51">
+    <row r="242" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>335</v>
       </c>
@@ -10207,7 +10214,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="178.5">
+    <row r="243" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>333</v>
       </c>
@@ -10233,7 +10240,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="89.25">
+    <row r="244" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>660</v>
       </c>
@@ -10259,7 +10266,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="38.25">
+    <row r="245" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>845</v>
       </c>
@@ -10285,7 +10292,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="38.25">
+    <row r="246" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>330</v>
       </c>
@@ -10311,7 +10318,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="76.5">
+    <row r="247" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>327</v>
       </c>
@@ -10337,7 +10344,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="38.25">
+    <row r="248" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>942</v>
       </c>
@@ -10363,7 +10370,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="38.25">
+    <row r="249" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>939</v>
       </c>
@@ -10389,7 +10396,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="38.25">
+    <row r="250" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>936</v>
       </c>
@@ -10415,7 +10422,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="63.75">
+    <row r="251" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>172</v>
       </c>
@@ -10441,7 +10448,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="89.25">
+    <row r="252" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>601</v>
       </c>
@@ -10467,7 +10474,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="89.25">
+    <row r="253" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>324</v>
       </c>
@@ -10493,7 +10500,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="63.75">
+    <row r="254" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>321</v>
       </c>
@@ -10519,7 +10526,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="89.25">
+    <row r="255" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>319</v>
       </c>
@@ -10545,7 +10552,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="38.25">
+    <row r="256" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>316</v>
       </c>
@@ -10571,7 +10578,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="38.25">
+    <row r="257" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>598</v>
       </c>
@@ -10597,7 +10604,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="76.5">
+    <row r="258" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>911</v>
       </c>
@@ -10623,7 +10630,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="38.25">
+    <row r="259" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>842</v>
       </c>
@@ -10649,7 +10656,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="38.25">
+    <row r="260" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>933</v>
       </c>
@@ -10675,7 +10682,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="38.25">
+    <row r="261" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>713</v>
       </c>
@@ -10701,7 +10708,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="51">
+    <row r="262" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>313</v>
       </c>
@@ -10727,7 +10734,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="38.25">
+    <row r="263" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>310</v>
       </c>
@@ -10753,7 +10760,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="51">
+    <row r="264" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>169</v>
       </c>
@@ -10779,7 +10786,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="51">
+    <row r="265" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>167</v>
       </c>
@@ -10805,7 +10812,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="51">
+    <row r="266" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>129</v>
       </c>
@@ -10831,7 +10838,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="63.75">
+    <row r="267" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>307</v>
       </c>
@@ -10857,7 +10864,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="178.5">
+    <row r="268" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>657</v>
       </c>
@@ -10883,7 +10890,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="38.25">
+    <row r="269" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>304</v>
       </c>
@@ -10909,7 +10916,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="51">
+    <row r="270" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>301</v>
       </c>
@@ -10935,7 +10942,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="51">
+    <row r="271" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>801</v>
       </c>
@@ -10961,7 +10968,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="165.75">
+    <row r="272" spans="1:8" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>798</v>
       </c>
@@ -10987,7 +10994,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="51">
+    <row r="273" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>30</v>
       </c>
@@ -11013,7 +11020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="51">
+    <row r="274" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>28</v>
       </c>
@@ -11039,7 +11046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="38.25">
+    <row r="275" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>298</v>
       </c>
@@ -11065,7 +11072,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="51">
+    <row r="276" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>295</v>
       </c>
@@ -11091,7 +11098,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="38.25">
+    <row r="277" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>292</v>
       </c>
@@ -11117,7 +11124,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="38.25">
+    <row r="278" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>930</v>
       </c>
@@ -11143,7 +11150,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="178.5">
+    <row r="279" spans="1:8" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>594</v>
       </c>
@@ -11169,7 +11176,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="89.25">
+    <row r="280" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>654</v>
       </c>
@@ -11195,7 +11202,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="281" spans="1:8" ht="51">
+    <row r="281" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>289</v>
       </c>
@@ -11221,7 +11228,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="51">
+    <row r="282" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>644</v>
       </c>
@@ -11247,7 +11254,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="38.25">
+    <row r="283" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>839</v>
       </c>
@@ -11273,7 +11280,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="284" spans="1:8" ht="63.75">
+    <row r="284" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>795</v>
       </c>
@@ -11299,7 +11306,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="285" spans="1:8" ht="51">
+    <row r="285" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>286</v>
       </c>
@@ -11325,7 +11332,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="38.25">
+    <row r="286" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>25</v>
       </c>
@@ -11351,7 +11358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:8" ht="51">
+    <row r="287" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>215</v>
       </c>
@@ -11377,7 +11384,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="288" spans="1:8" ht="38.25">
+    <row r="288" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>22</v>
       </c>
@@ -11403,7 +11410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="289" spans="1:8" ht="51">
+    <row r="289" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>927</v>
       </c>
@@ -11429,7 +11436,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="89.25">
+    <row r="290" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>164</v>
       </c>
@@ -11455,7 +11462,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="291" spans="1:8" ht="38.25">
+    <row r="291" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>924</v>
       </c>
@@ -11481,7 +11488,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="38.25">
+    <row r="292" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>710</v>
       </c>
@@ -11507,7 +11514,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="293" spans="1:8" ht="51">
+    <row r="293" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>820</v>
       </c>
@@ -11533,7 +11540,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="294" spans="1:8" ht="38.25">
+    <row r="294" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>19</v>
       </c>
@@ -11559,7 +11566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:8" ht="51">
+    <row r="295" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>651</v>
       </c>
@@ -11585,7 +11592,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="38.25">
+    <row r="296" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>921</v>
       </c>
@@ -11611,7 +11618,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="297" spans="1:8" ht="38.25">
+    <row r="297" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>707</v>
       </c>
@@ -11637,7 +11644,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="298" spans="1:8" ht="76.5">
+    <row r="298" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>817</v>
       </c>
@@ -11663,7 +11670,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="299" spans="1:8" ht="38.25">
+    <row r="299" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>704</v>
       </c>
@@ -11689,7 +11696,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="300" spans="1:8" ht="38.25">
+    <row r="300" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>126</v>
       </c>
@@ -11715,7 +11722,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="63.75">
+    <row r="301" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>637</v>
       </c>
@@ -11741,7 +11748,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="302" spans="1:8" ht="114.75">
+    <row r="302" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>547</v>
       </c>
@@ -11767,7 +11774,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="303" spans="1:8" ht="51">
+    <row r="303" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>545</v>
       </c>
@@ -11793,7 +11800,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="304" spans="1:8" ht="38.25">
+    <row r="304" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>918</v>
       </c>
@@ -11819,7 +11826,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="305" spans="1:8" ht="63.75">
+    <row r="305" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>701</v>
       </c>
@@ -11845,7 +11852,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="306" spans="1:8" ht="38.25">
+    <row r="306" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>554</v>
       </c>
@@ -11871,7 +11878,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="307" spans="1:8" ht="38.25">
+    <row r="307" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>551</v>
       </c>
@@ -11897,7 +11904,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="308" spans="1:8" ht="38.25">
+    <row r="308" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>283</v>
       </c>
@@ -11923,7 +11930,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="309" spans="1:8" ht="38.25">
+    <row r="309" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>915</v>
       </c>
@@ -11949,7 +11956,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="310" spans="1:8" ht="38.25">
+    <row r="310" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>280</v>
       </c>
@@ -11975,7 +11982,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="311" spans="1:8" ht="102">
+    <row r="311" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>277</v>
       </c>
@@ -12001,7 +12008,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="312" spans="1:8" ht="63.75">
+    <row r="312" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>908</v>
       </c>
@@ -12027,7 +12034,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="313" spans="1:8" ht="38.25">
+    <row r="313" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>906</v>
       </c>
@@ -12053,7 +12060,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="314" spans="1:8" ht="51">
+    <row r="314" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>698</v>
       </c>
@@ -12079,7 +12086,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="315" spans="1:8" ht="51">
+    <row r="315" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>273</v>
       </c>
@@ -12105,7 +12112,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="316" spans="1:8" ht="38.25">
+    <row r="316" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>695</v>
       </c>
@@ -12131,7 +12138,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="317" spans="1:8" ht="140.25">
+    <row r="317" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>270</v>
       </c>
@@ -12157,7 +12164,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="318" spans="1:8" ht="38.25">
+    <row r="318" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>267</v>
       </c>
@@ -12183,7 +12190,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="319" spans="1:8" ht="38.25">
+    <row r="319" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>634</v>
       </c>
@@ -12209,7 +12216,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="320" spans="1:8" ht="38.25">
+    <row r="320" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>632</v>
       </c>
@@ -12235,7 +12242,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="321" spans="1:8" ht="63.75">
+    <row r="321" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>264</v>
       </c>
@@ -12261,7 +12268,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="322" spans="1:8" ht="38.25">
+    <row r="322" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>221</v>
       </c>
@@ -12287,7 +12294,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="323" spans="1:8" ht="51">
+    <row r="323" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>219</v>
       </c>
@@ -12313,7 +12320,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="324" spans="1:8" ht="38.25">
+    <row r="324" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>261</v>
       </c>
@@ -12339,7 +12346,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="325" spans="1:8" ht="38.25">
+    <row r="325" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>258</v>
       </c>
@@ -12365,7 +12372,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="326" spans="1:8" ht="63.75">
+    <row r="326" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>692</v>
       </c>
@@ -12391,7 +12398,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="327" spans="1:8" ht="38.25">
+    <row r="327" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>255</v>
       </c>
@@ -12417,7 +12424,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="328" spans="1:8" ht="38.25">
+    <row r="328" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>836</v>
       </c>
@@ -12443,7 +12450,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="329" spans="1:8" ht="229.5">
+    <row r="329" spans="1:8" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>90</v>
       </c>
@@ -12469,7 +12476,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="330" spans="1:8" ht="51">
+    <row r="330" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>648</v>
       </c>
@@ -12495,7 +12502,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="331" spans="1:8" ht="38.25">
+    <row r="331" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>252</v>
       </c>

</xml_diff>